<commit_message>
Access files from github
</commit_message>
<xml_diff>
--- a/Data/test.xlsx
+++ b/Data/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinoestergaard/OneDrive/Documents/Skole/AU/ITKO/1. semester/DTIV/DTIV Test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinoestergaard/PycharmProjects/PreviewRecipe/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7596F269-9DF8-234D-AD24-08A05DDC9287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD66FE74-84CD-5343-BB6C-953E488C0A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="16340" xr2:uid="{AB5F43CE-F6A6-6342-9C2C-42983A56E8E8}"/>
   </bookViews>
@@ -36,18 +36,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>test123</t>
   </si>
   <si>
-    <t>test124</t>
+    <t>https://github.com/moestergaard/PreviewRecipe/blob/1f3ced3d6d066aa72005051d17a6839390de00e2/Data/pandekager.jpeg</t>
   </si>
   <si>
-    <t>test125</t>
+    <t>https://github.com/moestergaard/PreviewRecipe/blob/9f00694d6f0a79d43c26ae74f2a3fb6ec23c8178/Data/stegt-flaesk-med-persillesovs.jpeg</t>
   </si>
   <si>
-    <t>/Users/martinoestergaard/OneDrive/Documents/Skole/AU/ITKO/1. semester/DTIV/DTIV Test/pandekager.jpeg</t>
+    <t>Pandekager</t>
+  </si>
+  <si>
+    <t>Stegt Flæsk</t>
   </si>
 </sst>
 </file>
@@ -402,7 +405,7 @@
   <dimension ref="A2:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -420,7 +423,10 @@
         <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -428,10 +434,10 @@
         <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>